<commit_message>
created array in matlab
</commit_message>
<xml_diff>
--- a/ass2/data_g15.xlsx
+++ b/ass2/data_g15.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ArrivalTime" sheetId="1" r:id="rId1"/>
@@ -8143,10 +8143,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -8508,13 +8514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C805"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -17345,7 +17352,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -30246,7 +30255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B805"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>